<commit_message>
dda 7 anos, dda x5
</commit_message>
<xml_diff>
--- a/Datos_entrada_Internexa_21Jun18.xlsx
+++ b/Datos_entrada_Internexa_21Jun18.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576EDCB7-3500-41A2-A338-EE0D88BD7582}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC3A0F8-F93F-4EBF-A635-1DA6D1DA3D5A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="12210" tabRatio="809" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="12210" tabRatio="809" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TD m1_nodos" sheetId="10" state="hidden" r:id="rId1"/>
@@ -29,10 +29,10 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId12"/>
-    <pivotCache cacheId="4" r:id="rId13"/>
-    <pivotCache cacheId="5" r:id="rId14"/>
-    <pivotCache cacheId="6" r:id="rId15"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="1" r:id="rId13"/>
+    <pivotCache cacheId="2" r:id="rId14"/>
+    <pivotCache cacheId="3" r:id="rId15"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -6930,7 +6930,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" subtotalTop="0" showAll="0">
@@ -7080,7 +7080,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fases/Capacidad" colHeaderCaption="Fases">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fases/Capacidad" colHeaderCaption="Fases">
   <location ref="A3:B29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -7239,7 +7239,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A187218-2E9F-40EC-B039-D1C5902DF31E}" name="TablaDinámica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A187218-2E9F-40EC-B039-D1C5902DF31E}" name="TablaDinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F4:G29" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -7373,7 +7373,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000000000000}" name="TablaDinámica1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Capacidad KVA">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0500-000000000000}" name="TablaDinámica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Capacidad KVA">
   <location ref="A3:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -17022,8 +17022,8 @@
   </sheetPr>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17054,6 +17054,9 @@
       <c r="C2" s="2">
         <v>1200000</v>
       </c>
+      <c r="D2" s="17">
+        <v>1586217</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="18">
@@ -17079,6 +17082,9 @@
         <f t="shared" ref="C4:C9" si="0">C3*1.3</f>
         <v>2028000</v>
       </c>
+      <c r="D4" s="17">
+        <v>1831410</v>
+      </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:5">
@@ -17105,6 +17111,9 @@
         <f t="shared" si="0"/>
         <v>3427320</v>
       </c>
+      <c r="D6" s="17">
+        <v>2442086</v>
+      </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5">
@@ -17118,6 +17127,9 @@
         <f t="shared" si="0"/>
         <v>4455516</v>
       </c>
+      <c r="D7" s="17">
+        <v>2997610</v>
+      </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:5">
@@ -17131,6 +17143,9 @@
         <f t="shared" si="0"/>
         <v>5792170.7999999998</v>
       </c>
+      <c r="D8" s="17">
+        <v>3457763</v>
+      </c>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:5">
@@ -17144,6 +17159,9 @@
         <f t="shared" si="0"/>
         <v>7529822.04</v>
       </c>
+      <c r="D9" s="17">
+        <v>4458731</v>
+      </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:5">
@@ -17157,6 +17175,9 @@
         <f>C2*2.3</f>
         <v>2760000</v>
       </c>
+      <c r="D10" s="17">
+        <v>2979760</v>
+      </c>
       <c r="E10"/>
     </row>
     <row r="11" spans="1:5">
@@ -17183,6 +17204,9 @@
         <f t="shared" ref="C12:C22" si="1">C11*1.2</f>
         <v>3974400</v>
       </c>
+      <c r="D12" s="17">
+        <v>3514070</v>
+      </c>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:5">
@@ -17209,6 +17233,9 @@
         <f>C12*1.2</f>
         <v>4769280</v>
       </c>
+      <c r="D14" s="17">
+        <v>3951977</v>
+      </c>
       <c r="E14"/>
     </row>
     <row r="15" spans="1:5">
@@ -17248,6 +17275,9 @@
         <f>C15*1.2</f>
         <v>6867763.2000000002</v>
       </c>
+      <c r="D17" s="17">
+        <v>5041628</v>
+      </c>
       <c r="E17"/>
     </row>
     <row r="18" spans="1:5">
@@ -17260,6 +17290,9 @@
       <c r="C18" s="2">
         <f t="shared" si="1"/>
         <v>8241315.8399999999</v>
+      </c>
+      <c r="D18" s="17">
+        <v>5888415</v>
       </c>
       <c r="E18"/>
     </row>
@@ -34442,7 +34475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83115727-AD74-446E-A3AA-9EE0A33C0A75}">
   <dimension ref="B1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>

</xml_diff>